<commit_message>
qq fonctions changees et cr
</commit_message>
<xml_diff>
--- a/CR/horaires.xlsx
+++ b/CR/horaires.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="26100" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -45,18 +45,12 @@
     <t>Réalisation programme</t>
   </si>
   <si>
-    <t>test fns Matlab</t>
-  </si>
-  <si>
     <t>Incorporation fns Matlab</t>
   </si>
   <si>
     <t>Mise en place Github</t>
   </si>
   <si>
-    <t>Fns de traitement initial</t>
-  </si>
-  <si>
     <t>Détection de contours</t>
   </si>
   <si>
@@ -81,17 +75,23 @@
     <t>Rédaction Compte rendu</t>
   </si>
   <si>
-    <t>ajout logs, automatisme</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Familiarisation avec fonctions</t>
+  </si>
+  <si>
+    <t>Fonctions de traitement initial</t>
+  </si>
+  <si>
+    <t>test fonctions Matlab</t>
+  </si>
+  <si>
+    <t>Ajout logs, automatisme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +99,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -125,22 +139,130 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,31 +564,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:I28"/>
+  <dimension ref="A5:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>42675</v>
       </c>
       <c r="D5" s="2">
@@ -484,251 +606,251 @@
       <c r="H5" s="2">
         <v>42709</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>42716</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="4" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="E16" s="4" t="s">
+    </row>
+    <row r="20" spans="3:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="3:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="G21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="H18" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="H20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="F22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -741,7 +863,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -753,7 +875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>